<commit_message>
updating branch from github
</commit_message>
<xml_diff>
--- a/Data from 11.18.21/eso.xlsx
+++ b/Data from 11.18.21/eso.xlsx
@@ -6472,8 +6472,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E6F65F02304A9EFDC2289E2E3833" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a49a311a0a0f87ea3ff4d334848598e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="446029cd-d925-4579-bf5d-30ef27c8be74" xmlns:ns3="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98345c2186b81bf10bf742872e889296" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004456E6F65F02304A9EFDC2289E2E3833" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99f380d18f3f307f6411cd7d315e286c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="446029cd-d925-4579-bf5d-30ef27c8be74" xmlns:ns3="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b51c68ca466ebae82acd68775f0ee2e" ns2:_="" ns3:_="">
     <xsd:import namespace="446029cd-d925-4579-bf5d-30ef27c8be74"/>
     <xsd:import namespace="a883631d-14a9-4c29-9489-4cf8dfc7ddfa"/>
     <xsd:element name="properties">
@@ -6493,6 +6493,9 @@
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -6552,6 +6555,18 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="19" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="f7310ada-04f1-49d1-83c9-5a60708465d1" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -6581,6 +6596,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{96d1ae44-0ed9-4cca-9b02-f09f4d28eadf}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="a883631d-14a9-4c29-9489-4cf8dfc7ddfa">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -6693,12 +6719,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="446029cd-d925-4579-bf5d-30ef27c8be74">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a883631d-14a9-4c29-9489-4cf8dfc7ddfa" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA203F2-6194-4782-B8E2-7A5F317D4867}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB972D87-2D25-4695-8DAE-B9F44BDE2BBC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>